<commit_message>
Add pipeline pic and finalize files
</commit_message>
<xml_diff>
--- a/GIT&GITHUB.xlsx
+++ b/GIT&GITHUB.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Munka3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -805,13 +804,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -822,22 +856,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -845,26 +865,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -872,11 +877,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,6 +887,49 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2444751</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>129886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4826001</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>209465</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Kép 1" descr="git_pipeline.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2444751" y="35435886"/>
+          <a:ext cx="7397750" cy="4127704"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1172,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B148"/>
+  <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A113" zoomScale="60" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A120" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1186,10 +1231,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
@@ -1288,10 +1333,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="20.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
@@ -1326,16 +1371,16 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="21" thickBot="1">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="27"/>
+      <c r="B21" s="16"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="17" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1343,19 +1388,19 @@
       <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="11"/>
+      <c r="B23" s="17"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="11"/>
+      <c r="B24" s="17"/>
     </row>
     <row r="26" spans="1:2" ht="21" thickBot="1">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="27"/>
+      <c r="B26" s="16"/>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
@@ -1374,13 +1419,13 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="21" thickBot="1">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="27"/>
+      <c r="B30" s="16"/>
     </row>
     <row r="31" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="28" t="s">
         <v>45</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1388,10 +1433,10 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="21" thickBot="1">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="27"/>
+      <c r="B33" s="16"/>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
@@ -1426,10 +1471,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="21" thickBot="1">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="27"/>
+      <c r="B39" s="16"/>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
@@ -1456,10 +1501,10 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="21" thickBot="1">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="27"/>
+      <c r="B44" s="16"/>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
@@ -1494,8 +1539,8 @@
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="13"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2" t="s">
@@ -1530,8 +1575,8 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="13"/>
-      <c r="B54" s="12"/>
+      <c r="A54" s="6"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
@@ -1550,8 +1595,8 @@
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="13"/>
-      <c r="B57" s="12"/>
+      <c r="A57" s="6"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
@@ -1562,10 +1607,10 @@
       </c>
     </row>
     <row r="60" spans="1:2" ht="21" thickBot="1">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B60" s="27"/>
+      <c r="B60" s="16"/>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
@@ -1576,22 +1621,22 @@
       </c>
     </row>
     <row r="63" spans="1:2" ht="21" thickBot="1">
-      <c r="A63" s="26" t="s">
+      <c r="A63" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="27"/>
+      <c r="B63" s="16"/>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="18" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="7"/>
-      <c r="B65" s="6"/>
+      <c r="A65" s="20"/>
+      <c r="B65" s="19"/>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2" t="s">
@@ -1634,10 +1679,10 @@
       </c>
     </row>
     <row r="72" spans="1:2" ht="21" thickBot="1">
-      <c r="A72" s="26" t="s">
+      <c r="A72" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B72" s="27"/>
+      <c r="B72" s="16"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2" t="s">
@@ -1696,10 +1741,10 @@
       </c>
     </row>
     <row r="81" spans="1:2" ht="21" thickBot="1">
-      <c r="A81" s="26" t="s">
+      <c r="A81" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B81" s="27"/>
+      <c r="B81" s="16"/>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2" t="s">
@@ -1710,16 +1755,16 @@
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="21" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="7"/>
-      <c r="B84" s="9"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="21"/>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2" t="s">
@@ -1738,8 +1783,8 @@
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="13"/>
-      <c r="B87" s="12"/>
+      <c r="A87" s="6"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2" t="s">
@@ -1750,8 +1795,8 @@
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="13"/>
-      <c r="B89" s="12"/>
+      <c r="A89" s="6"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2" t="s">
@@ -1778,8 +1823,8 @@
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="13"/>
-      <c r="B93" s="12"/>
+      <c r="A93" s="6"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2" t="s">
@@ -1798,8 +1843,8 @@
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="13"/>
-      <c r="B96" s="12"/>
+      <c r="A96" s="6"/>
+      <c r="B96" s="5"/>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2" t="s">
@@ -1810,33 +1855,33 @@
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="10" t="s">
+      <c r="A99" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="B99" s="10"/>
+      <c r="B99" s="13"/>
     </row>
     <row r="100" spans="1:2" ht="21" thickBot="1">
-      <c r="A100" s="26" t="s">
+      <c r="A100" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B100" s="27"/>
+      <c r="B100" s="16"/>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="B101" s="7" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="21" thickBot="1">
-      <c r="A103" s="26" t="s">
+      <c r="A103" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B103" s="27"/>
+      <c r="B103" s="16"/>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="21" t="s">
+      <c r="A104" s="11" t="s">
         <v>140</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -1844,7 +1889,7 @@
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="21" t="s">
+      <c r="A105" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -1852,7 +1897,7 @@
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="21" t="s">
+      <c r="A106" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -1860,7 +1905,7 @@
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="21" t="s">
+      <c r="A107" s="11" t="s">
         <v>143</v>
       </c>
       <c r="B107" s="3" t="s">
@@ -1868,7 +1913,7 @@
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="21" t="s">
+      <c r="A108" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -1876,10 +1921,10 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="21" thickBot="1">
-      <c r="A110" s="26" t="s">
+      <c r="A110" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B110" s="27"/>
+      <c r="B110" s="16"/>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="2" t="s">
@@ -1906,25 +1951,25 @@
       </c>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" s="7" t="s">
+      <c r="A114" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="B114" s="15" t="s">
+      <c r="B114" s="22" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" s="7"/>
-      <c r="B115" s="16"/>
+      <c r="A115" s="20"/>
+      <c r="B115" s="23"/>
     </row>
     <row r="116" spans="1:2">
-      <c r="B116" s="17"/>
+      <c r="B116" s="8"/>
     </row>
     <row r="117" spans="1:2" ht="21" thickBot="1">
-      <c r="A117" s="26" t="s">
+      <c r="A117" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B117" s="27"/>
+      <c r="B117" s="16"/>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="2" t="s">
@@ -1935,71 +1980,71 @@
       </c>
     </row>
     <row r="119" spans="1:2">
-      <c r="A119" s="7" t="s">
+      <c r="A119" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="B119" s="18" t="s">
+      <c r="B119" s="24" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="120" spans="1:2">
-      <c r="A120" s="7"/>
-      <c r="B120" s="18"/>
+      <c r="A120" s="20"/>
+      <c r="B120" s="24"/>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="7" t="s">
+      <c r="A121" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="B121" s="18" t="s">
+      <c r="B121" s="24" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="122" spans="1:2">
-      <c r="A122" s="7"/>
-      <c r="B122" s="18"/>
+      <c r="A122" s="20"/>
+      <c r="B122" s="24"/>
     </row>
     <row r="123" spans="1:2">
-      <c r="A123" s="19"/>
-      <c r="B123" s="19"/>
+      <c r="A123" s="9"/>
+      <c r="B123" s="9"/>
     </row>
     <row r="124" spans="1:2" ht="21" thickBot="1">
-      <c r="A124" s="26" t="s">
+      <c r="A124" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B124" s="27"/>
+      <c r="B124" s="16"/>
     </row>
     <row r="125" spans="1:2">
-      <c r="A125" s="22" t="s">
+      <c r="A125" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="B125" s="18" t="s">
+      <c r="B125" s="24" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="126" spans="1:2">
-      <c r="A126" s="22"/>
-      <c r="B126" s="18"/>
+      <c r="A126" s="25"/>
+      <c r="B126" s="24"/>
     </row>
     <row r="127" spans="1:2">
-      <c r="A127" s="7" t="s">
+      <c r="A127" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B127" s="18" t="s">
+      <c r="B127" s="24" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="128" spans="1:2">
-      <c r="A128" s="7"/>
-      <c r="B128" s="18"/>
+      <c r="A128" s="20"/>
+      <c r="B128" s="24"/>
     </row>
     <row r="130" spans="1:2" ht="21" thickBot="1">
-      <c r="A130" s="26" t="s">
+      <c r="A130" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="B130" s="27"/>
+      <c r="B130" s="16"/>
     </row>
     <row r="131" spans="1:2">
-      <c r="A131" s="21" t="s">
+      <c r="A131" s="11" t="s">
         <v>168</v>
       </c>
       <c r="B131" s="3" t="s">
@@ -2007,7 +2052,7 @@
       </c>
     </row>
     <row r="132" spans="1:2">
-      <c r="A132" s="21" t="s">
+      <c r="A132" s="11" t="s">
         <v>169</v>
       </c>
       <c r="B132" s="3" t="s">
@@ -2015,11 +2060,11 @@
       </c>
     </row>
     <row r="133" spans="1:2">
-      <c r="A133" s="13"/>
-      <c r="B133" s="12"/>
+      <c r="A133" s="6"/>
+      <c r="B133" s="5"/>
     </row>
     <row r="134" spans="1:2">
-      <c r="A134" s="21" t="s">
+      <c r="A134" s="11" t="s">
         <v>170</v>
       </c>
       <c r="B134" s="3" t="s">
@@ -2027,7 +2072,7 @@
       </c>
     </row>
     <row r="135" spans="1:2">
-      <c r="A135" s="21" t="s">
+      <c r="A135" s="11" t="s">
         <v>171</v>
       </c>
       <c r="B135" s="3" t="s">
@@ -2035,11 +2080,11 @@
       </c>
     </row>
     <row r="136" spans="1:2">
-      <c r="A136" s="13"/>
-      <c r="B136" s="12"/>
+      <c r="A136" s="6"/>
+      <c r="B136" s="5"/>
     </row>
     <row r="137" spans="1:2">
-      <c r="A137" s="21" t="s">
+      <c r="A137" s="11" t="s">
         <v>172</v>
       </c>
       <c r="B137" s="3" t="s">
@@ -2047,7 +2092,7 @@
       </c>
     </row>
     <row r="138" spans="1:2">
-      <c r="A138" s="21" t="s">
+      <c r="A138" s="11" t="s">
         <v>173</v>
       </c>
       <c r="B138" s="3" t="s">
@@ -2055,7 +2100,7 @@
       </c>
     </row>
     <row r="139" spans="1:2">
-      <c r="A139" s="21" t="s">
+      <c r="A139" s="11" t="s">
         <v>174</v>
       </c>
       <c r="B139" s="3" t="s">
@@ -2063,7 +2108,7 @@
       </c>
     </row>
     <row r="140" spans="1:2">
-      <c r="A140" s="21" t="s">
+      <c r="A140" s="11" t="s">
         <v>175</v>
       </c>
       <c r="B140" s="3" t="s">
@@ -2071,11 +2116,11 @@
       </c>
     </row>
     <row r="141" spans="1:2">
-      <c r="A141" s="23"/>
-      <c r="B141" s="12"/>
+      <c r="A141" s="12"/>
+      <c r="B141" s="5"/>
     </row>
     <row r="142" spans="1:2">
-      <c r="A142" s="21" t="s">
+      <c r="A142" s="11" t="s">
         <v>176</v>
       </c>
       <c r="B142" s="3" t="s">
@@ -2083,23 +2128,23 @@
       </c>
     </row>
     <row r="143" spans="1:2">
-      <c r="A143" s="23"/>
-      <c r="B143" s="12"/>
+      <c r="A143" s="12"/>
+      <c r="B143" s="5"/>
     </row>
     <row r="144" spans="1:2">
-      <c r="A144" s="22" t="s">
+      <c r="A144" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="B144" s="18" t="s">
+      <c r="B144" s="24" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="145" spans="1:2">
-      <c r="A145" s="22"/>
-      <c r="B145" s="18"/>
+      <c r="A145" s="25"/>
+      <c r="B145" s="24"/>
     </row>
     <row r="146" spans="1:2">
-      <c r="A146" s="21" t="s">
+      <c r="A146" s="11" t="s">
         <v>178</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -2107,42 +2152,37 @@
       </c>
     </row>
     <row r="147" spans="1:2">
-      <c r="A147" s="20"/>
-    </row>
-    <row r="148" spans="1:2" ht="20.25">
-      <c r="A148" s="24" t="s">
+      <c r="A147" s="10"/>
+    </row>
+    <row r="165" spans="1:2" ht="20.25">
+      <c r="A165" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="B148" s="25"/>
+      <c r="B165" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="37">
     <mergeCell ref="A144:A145"/>
     <mergeCell ref="B144:B145"/>
-    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A165:B165"/>
     <mergeCell ref="A117:B117"/>
     <mergeCell ref="A124:B124"/>
     <mergeCell ref="A130:B130"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="B127:B128"/>
     <mergeCell ref="B114:B115"/>
     <mergeCell ref="A114:A115"/>
     <mergeCell ref="B119:B120"/>
     <mergeCell ref="A119:A120"/>
     <mergeCell ref="B121:B122"/>
     <mergeCell ref="A121:A122"/>
-    <mergeCell ref="B125:B126"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="B127:B128"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A99:B99"/>
     <mergeCell ref="A100:B100"/>
     <mergeCell ref="A103:B103"/>
     <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A44:B44"/>
@@ -2154,13 +2194,21 @@
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="B83:B84"/>
     <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="73" fitToHeight="4" orientation="portrait" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="70" max="16383" man="1"/>
+  <pageSetup paperSize="8" scale="99" fitToHeight="4" orientation="landscape" r:id="rId1"/>
+  <rowBreaks count="3" manualBreakCount="3">
+    <brk id="43" max="16383" man="1"/>
+    <brk id="80" max="16383" man="1"/>
+    <brk id="165" max="16383" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>